<commit_message>
Update bai 2 va bai 3
</commit_message>
<xml_diff>
--- a/Bai 2-Giai phuong trinh bac 2.xlsx
+++ b/Bai 2-Giai phuong trinh bac 2.xlsx
@@ -282,10 +282,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3022,7 +3022,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>STAR</a:t>
+            <a:t>STOP</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3494,7 +3494,7 @@
   <dimension ref="B1:Y37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3504,23 +3504,23 @@
   <sheetData>
     <row r="1" spans="2:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -3532,21 +3532,21 @@
       <c r="Y2" s="1"/>
     </row>
     <row r="3" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -3558,21 +3558,21 @@
       <c r="Y3" s="1"/>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -3584,21 +3584,21 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -3610,21 +3610,21 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -3636,21 +3636,21 @@
       <c r="Y6" s="1"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -3662,21 +3662,21 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -3688,21 +3688,21 @@
       <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -3714,21 +3714,21 @@
       <c r="Y9" s="1"/>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -3740,21 +3740,21 @@
       <c r="Y10" s="1"/>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -3766,21 +3766,21 @@
       <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -3792,21 +3792,21 @@
       <c r="Y12" s="1"/>
     </row>
     <row r="13" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -3818,21 +3818,21 @@
       <c r="Y13" s="1"/>
     </row>
     <row r="14" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -3844,21 +3844,21 @@
       <c r="Y14" s="1"/>
     </row>
     <row r="15" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -3870,21 +3870,21 @@
       <c r="Y15" s="1"/>
     </row>
     <row r="16" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -3896,21 +3896,21 @@
       <c r="Y16" s="1"/>
     </row>
     <row r="17" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -3922,21 +3922,21 @@
       <c r="Y17" s="1"/>
     </row>
     <row r="18" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -3948,21 +3948,21 @@
       <c r="Y18" s="1"/>
     </row>
     <row r="19" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -3974,21 +3974,21 @@
       <c r="Y19" s="1"/>
     </row>
     <row r="20" spans="2:25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -4000,21 +4000,21 @@
       <c r="Y20" s="1"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -4026,21 +4026,21 @@
       <c r="Y21" s="1"/>
     </row>
     <row r="22" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -4052,21 +4052,21 @@
       <c r="Y22" s="1"/>
     </row>
     <row r="23" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -4078,21 +4078,21 @@
       <c r="Y23" s="1"/>
     </row>
     <row r="24" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -4104,225 +4104,225 @@
       <c r="Y24" s="1"/>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>